<commit_message>
University finished, added bottle model,  Ui update, lightning update
-University is now finished. Exams added, all activities added etc (code must be cleaned up).
-UI has now grid mode almost all panels
-Bottle model added (no code for relating inventory with bottles in the fridge yet)
-Lightning improved, changed global light, added fridge and lamp light
-Change light intensity depended on the time
</commit_message>
<xml_diff>
--- a/prog-tycoon/Assets/prog-tycoon-numbers.xlsx
+++ b/prog-tycoon/Assets/prog-tycoon-numbers.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubek\Documents\GitHub\Prog-tycoon\prog-tycoon\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077DCA06-A4C0-4241-B1ED-508888769834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666F2A9A-4FA4-4D88-9FBF-AFBAA6CB8C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="6360" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skills" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Basic skills</t>
   </si>
@@ -73,13 +84,22 @@
   </si>
   <si>
     <t>C++</t>
+  </si>
+  <si>
+    <t>Time:</t>
+  </si>
+  <si>
+    <t>Result for &gt;4</t>
+  </si>
+  <si>
+    <t>Result for &lt;4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +130,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC678DD"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -131,11 +158,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -416,19 +446,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -444,7 +475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -452,7 +483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -460,7 +491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -468,7 +499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -476,7 +507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -484,12 +515,38 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="4">
+        <f>0.01+(J10/(100/J10*J10*J10*J10))</f>
+        <v>1.125E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="4">
+        <f>0.01+(J10/(100/J10*J10))</f>
+        <v>0.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>